<commit_message>
New schedule + html files
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
   <si>
     <t>Poll "Presenting solutions for the problem sets"</t>
   </si>
@@ -248,6 +248,18 @@
   </si>
   <si>
     <t>Patrick Pöpperling (with Katrin Marques and Marc Kerstan)</t>
+  </si>
+  <si>
+    <t>Nargiz Ahmadova (007)</t>
+  </si>
+  <si>
+    <t>Altaf Hussain</t>
+  </si>
+  <si>
+    <t>Valentyn Khmarskyi</t>
+  </si>
+  <si>
+    <t>Ozodbek Ozodov</t>
   </si>
 </sst>
 </file>
@@ -317,7 +329,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -430,13 +442,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -478,6 +510,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -639,13 +680,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -735,19 +770,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1002,13 +1037,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1312,19 +1341,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1575,7 +1604,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2440,6 +2469,70 @@
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
     </row>
+    <row r="53" ht="13.65" customHeight="1">
+      <c r="A53" t="s" s="14">
+        <v>79</v>
+      </c>
+      <c r="B53" s="12"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
+      <c r="J53" t="s" s="13">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" ht="13.65" customHeight="1">
+      <c r="A54" t="s" s="15">
+        <v>80</v>
+      </c>
+      <c r="B54" s="12"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" t="s" s="13">
+        <v>16</v>
+      </c>
+      <c r="J54" s="12"/>
+    </row>
+    <row r="55" ht="13.65" customHeight="1">
+      <c r="A55" t="s" s="16">
+        <v>81</v>
+      </c>
+      <c r="B55" s="12"/>
+      <c r="C55" s="13"/>
+      <c r="D55" t="s" s="13">
+        <v>44</v>
+      </c>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+    </row>
+    <row r="56" ht="13.65" customHeight="1">
+      <c r="A56" t="s" s="16">
+        <v>82</v>
+      </c>
+      <c r="B56" s="12"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" t="s" s="13">
+        <v>71</v>
+      </c>
+      <c r="I56" s="12"/>
+      <c r="J56" s="12"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B4:C4"/>

</xml_diff>